<commit_message>
mudei escala do plot metareg qualidade
</commit_message>
<xml_diff>
--- a/data/influence2.xlsx
+++ b/data/influence2.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://ufscbr-my.sharepoint.com/personal/tamires_martins_ufsc_br/Documents/PC LAB/DissAnalysis/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="15" documentId="11_3363FFC68F79A8D366075C52F37BD2721AC2F787" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{4E7BB37D-069B-4E96-9723-7CA3CCC4FBB9}"/>
+  <xr:revisionPtr revIDLastSave="16" documentId="11_3363FFC68F79A8D366075C52F37BD2721AC2F787" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{1307EAF8-EB69-43A0-88C9-9A8014DB15DD}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="20370" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1729" uniqueCount="790">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1729" uniqueCount="794">
   <si>
     <t>rstudent</t>
   </si>
@@ -2350,53 +2350,65 @@
     <t xml:space="preserve"> </t>
   </si>
   <si>
-    <t>water depth 8 cm, persa</t>
-  </si>
-  <si>
-    <t>persa</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> no strain reported, pretest mice</t>
-  </si>
-  <si>
-    <t>pretest mice</t>
-  </si>
-  <si>
-    <t>10/14, other studies from this publication also used this light regime, but for this comparsons the immobility time of vehicle was higher</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> F, ovariectomized, subcutaneous</t>
-  </si>
-  <si>
-    <t>CUMs</t>
-  </si>
-  <si>
-    <t>-</t>
-  </si>
-  <si>
-    <t>erro na escala, corrigi na planilha crua</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> stress reserpine</t>
-  </si>
-  <si>
-    <t>water depth 8 cm</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> sex? no info bioterium and duration of tratement</t>
-  </si>
-  <si>
-    <t>laca</t>
-  </si>
-  <si>
-    <t>erro tem stress, corrigi na planilha crua</t>
+    <t xml:space="preserve">water depth 8 cm, persa, quali 4 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">persa, quali 4 </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> no strain reported, pretest mice, quali 1</t>
+  </si>
+  <si>
+    <t>pretest mice, quali 5</t>
+  </si>
+  <si>
+    <t>10/14, other studies from this publication also used this light regime, but for this comparsons the immobility time of vehicle was higher, quali 5</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> F, ovariectomized, subcutaneous, quali 5</t>
+  </si>
+  <si>
+    <t>CUMs, quali 4</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> quali 3</t>
+  </si>
+  <si>
+    <t>quali 3</t>
+  </si>
+  <si>
+    <t>quali 4</t>
+  </si>
+  <si>
+    <t>erro na escala, corrigi na planilha crua, quali 4</t>
+  </si>
+  <si>
+    <t>pretest mice, quali 4</t>
+  </si>
+  <si>
+    <t>stress reserpine, quali 3</t>
+  </si>
+  <si>
+    <t>water depth 8 cm, quali 5</t>
+  </si>
+  <si>
+    <t>quali 5</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> sex? no info bioterium and duration of tratement, quali 4</t>
+  </si>
+  <si>
+    <t>laca, quali 4</t>
+  </si>
+  <si>
+    <t>erro tem stress, corrigi na planilha crua, quali 5</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -2408,6 +2420,12 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -2779,8 +2797,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:M562"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L291" sqref="L291"/>
+    <sheetView tabSelected="1" topLeftCell="A547" workbookViewId="0">
+      <selection activeCell="M558" sqref="M558"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8445,7 +8463,7 @@
         <v>223</v>
       </c>
       <c r="M148" t="s">
-        <v>783</v>
+        <v>784</v>
       </c>
     </row>
     <row r="149" spans="1:13" x14ac:dyDescent="0.25">
@@ -8486,7 +8504,7 @@
         <v>223</v>
       </c>
       <c r="M149" t="s">
-        <v>783</v>
+        <v>784</v>
       </c>
     </row>
     <row r="150" spans="1:13" x14ac:dyDescent="0.25">
@@ -10845,7 +10863,7 @@
         <v>305</v>
       </c>
       <c r="M211" t="s">
-        <v>784</v>
+        <v>786</v>
       </c>
     </row>
     <row r="212" spans="1:13" x14ac:dyDescent="0.25">
@@ -11684,7 +11702,7 @@
         <v>339</v>
       </c>
       <c r="M233" t="s">
-        <v>785</v>
+        <v>788</v>
       </c>
     </row>
     <row r="234" spans="1:13" x14ac:dyDescent="0.25">
@@ -12105,7 +12123,7 @@
         <v>351</v>
       </c>
       <c r="M244" t="s">
-        <v>779</v>
+        <v>787</v>
       </c>
     </row>
     <row r="245" spans="1:13" x14ac:dyDescent="0.25">
@@ -13780,7 +13798,7 @@
         <v>403</v>
       </c>
       <c r="M288" t="s">
-        <v>779</v>
+        <v>787</v>
       </c>
     </row>
     <row r="289" spans="1:13" x14ac:dyDescent="0.25">
@@ -13821,7 +13839,7 @@
         <v>403</v>
       </c>
       <c r="M289" t="s">
-        <v>779</v>
+        <v>787</v>
       </c>
     </row>
     <row r="290" spans="1:13" x14ac:dyDescent="0.25">
@@ -13862,7 +13880,7 @@
         <v>403</v>
       </c>
       <c r="M290" t="s">
-        <v>779</v>
+        <v>787</v>
       </c>
     </row>
     <row r="291" spans="1:13" x14ac:dyDescent="0.25">
@@ -13903,7 +13921,7 @@
         <v>411</v>
       </c>
       <c r="M291" t="s">
-        <v>786</v>
+        <v>789</v>
       </c>
     </row>
     <row r="292" spans="1:13" x14ac:dyDescent="0.25">
@@ -14704,7 +14722,7 @@
         <v>441</v>
       </c>
       <c r="M312" t="s">
-        <v>783</v>
+        <v>785</v>
       </c>
     </row>
     <row r="313" spans="1:13" x14ac:dyDescent="0.25">
@@ -14821,7 +14839,7 @@
         <v>441</v>
       </c>
       <c r="M315" t="s">
-        <v>783</v>
+        <v>785</v>
       </c>
     </row>
     <row r="316" spans="1:13" x14ac:dyDescent="0.25">
@@ -15090,7 +15108,7 @@
         <v>456</v>
       </c>
       <c r="M322" t="s">
-        <v>783</v>
+        <v>785</v>
       </c>
     </row>
     <row r="323" spans="1:13" x14ac:dyDescent="0.25">
@@ -15131,7 +15149,7 @@
         <v>456</v>
       </c>
       <c r="M323" t="s">
-        <v>783</v>
+        <v>785</v>
       </c>
     </row>
     <row r="324" spans="1:13" x14ac:dyDescent="0.25">
@@ -15172,7 +15190,7 @@
         <v>456</v>
       </c>
       <c r="M324" t="s">
-        <v>783</v>
+        <v>785</v>
       </c>
     </row>
     <row r="325" spans="1:13" x14ac:dyDescent="0.25">
@@ -15213,7 +15231,7 @@
         <v>456</v>
       </c>
       <c r="M325" t="s">
-        <v>783</v>
+        <v>785</v>
       </c>
     </row>
     <row r="326" spans="1:13" x14ac:dyDescent="0.25">
@@ -15254,7 +15272,7 @@
         <v>456</v>
       </c>
       <c r="M326" t="s">
-        <v>783</v>
+        <v>785</v>
       </c>
     </row>
     <row r="327" spans="1:13" x14ac:dyDescent="0.25">
@@ -15447,7 +15465,7 @@
         <v>467</v>
       </c>
       <c r="M331" t="s">
-        <v>783</v>
+        <v>790</v>
       </c>
     </row>
     <row r="332" spans="1:13" x14ac:dyDescent="0.25">
@@ -15488,7 +15506,7 @@
         <v>467</v>
       </c>
       <c r="M332" t="s">
-        <v>783</v>
+        <v>790</v>
       </c>
     </row>
     <row r="333" spans="1:13" x14ac:dyDescent="0.25">
@@ -16213,7 +16231,7 @@
         <v>498</v>
       </c>
       <c r="M351" t="s">
-        <v>787</v>
+        <v>791</v>
       </c>
     </row>
     <row r="352" spans="1:13" x14ac:dyDescent="0.25">
@@ -16824,7 +16842,7 @@
         <v>518</v>
       </c>
       <c r="M367" t="s">
-        <v>788</v>
+        <v>792</v>
       </c>
     </row>
     <row r="368" spans="1:13" x14ac:dyDescent="0.25">
@@ -21197,7 +21215,7 @@
         <v>667</v>
       </c>
       <c r="M482" t="s">
-        <v>783</v>
+        <v>785</v>
       </c>
     </row>
     <row r="483" spans="1:13" x14ac:dyDescent="0.25">
@@ -21732,7 +21750,7 @@
         <v>685</v>
       </c>
       <c r="M496" t="s">
-        <v>789</v>
+        <v>793</v>
       </c>
     </row>
     <row r="497" spans="1:13" x14ac:dyDescent="0.25">
@@ -24244,6 +24262,7 @@
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>